<commit_message>
Read.py [Last read from reader]
</commit_message>
<xml_diff>
--- a/parking_lot.xlsx
+++ b/parking_lot.xlsx
@@ -512,10 +512,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>589090</v>

</xml_diff>

<commit_message>
Read.py [Connected and Ready]
</commit_message>
<xml_diff>
--- a/parking_lot.xlsx
+++ b/parking_lot.xlsx
@@ -512,10 +512,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>589090</v>

</xml_diff>

<commit_message>
Read.py [No tag, reader active]
</commit_message>
<xml_diff>
--- a/parking_lot.xlsx
+++ b/parking_lot.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
     <t>Parking Spot</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>n</t>
-  </si>
-  <si>
-    <t>y</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Read.py [Connected, reader active]
</commit_message>
<xml_diff>
--- a/parking_lot.xlsx
+++ b/parking_lot.xlsx
@@ -14,21 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>Parking Spot</t>
   </si>
   <si>
-    <t>Occupied</t>
-  </si>
-  <si>
-    <t>Registered</t>
+    <t>n</t>
   </si>
   <si>
     <t>Student ID</t>
-  </si>
-  <si>
-    <t>n</t>
   </si>
   <si>
     <t>y</t>
@@ -434,14 +428,14 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="2" t="b">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="E1" s="3" t="n">
         <v>42806.0773459827</v>
@@ -456,7 +450,7 @@
         <v/>
       </c>
       <c r="C2" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="n">
         <v>123456</v>
@@ -471,7 +465,7 @@
         <v/>
       </c>
       <c r="C3" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="n">
         <v>234567</v>
@@ -486,7 +480,7 @@
         <v/>
       </c>
       <c r="C4" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="n">
         <v>345678</v>
@@ -501,7 +495,7 @@
         <v/>
       </c>
       <c r="C5" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="n">
         <v>456789</v>
@@ -515,7 +509,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D6" s="2" t="n">
         <v>589090</v>
@@ -530,7 +524,7 @@
         <v/>
       </c>
       <c r="C7" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="n">
         <v>987654</v>
@@ -545,7 +539,7 @@
         <v/>
       </c>
       <c r="C8" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="n">
         <v>876543</v>
@@ -560,7 +554,7 @@
         <v/>
       </c>
       <c r="C9" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="n">
         <v>765432</v>
@@ -575,7 +569,7 @@
         <v/>
       </c>
       <c r="C10" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>654321</v>
@@ -590,7 +584,7 @@
         <v/>
       </c>
       <c r="C11" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="n">
         <v>159357</v>
@@ -605,7 +599,7 @@
         <v/>
       </c>
       <c r="C12" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="n">
         <v>456852</v>
@@ -620,7 +614,7 @@
         <v/>
       </c>
       <c r="C13" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>357159</v>
@@ -635,7 +629,7 @@
         <v/>
       </c>
       <c r="C14" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="n">
         <v>0</v>
@@ -650,7 +644,7 @@
         <v/>
       </c>
       <c r="C15" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>0</v>
@@ -665,7 +659,7 @@
         <v/>
       </c>
       <c r="C16" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="n">
         <v>0</v>
@@ -680,7 +674,7 @@
         <v/>
       </c>
       <c r="C17" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="n">
         <v>0</v>
@@ -695,7 +689,7 @@
         <v/>
       </c>
       <c r="C18" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="n">
         <v>0</v>
@@ -710,7 +704,7 @@
         <v/>
       </c>
       <c r="C19" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="n">
         <v>0</v>
@@ -725,7 +719,7 @@
         <v/>
       </c>
       <c r="C20" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="n">
         <v>0</v>
@@ -740,7 +734,7 @@
         <v/>
       </c>
       <c r="C21" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="n">
         <v>0</v>
@@ -755,7 +749,7 @@
         <v/>
       </c>
       <c r="C22" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="n">
         <v>0</v>
@@ -770,7 +764,7 @@
         <v/>
       </c>
       <c r="C23" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="n">
         <v>0</v>
@@ -785,7 +779,7 @@
         <v/>
       </c>
       <c r="C24" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="n">
         <v>0</v>
@@ -800,7 +794,7 @@
         <v/>
       </c>
       <c r="C25" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2" t="n">
         <v>0</v>
@@ -815,7 +809,7 @@
         <v/>
       </c>
       <c r="C26" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D26" s="2" t="n">
         <v>0</v>
@@ -830,7 +824,7 @@
         <v/>
       </c>
       <c r="C27" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D27" s="2" t="n">
         <v>0</v>
@@ -845,7 +839,7 @@
         <v/>
       </c>
       <c r="C28" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D28" s="2" t="n">
         <v>0</v>
@@ -860,7 +854,7 @@
         <v/>
       </c>
       <c r="C29" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D29" s="2" t="n">
         <v>0</v>
@@ -875,7 +869,7 @@
         <v/>
       </c>
       <c r="C30" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D30" s="2" t="n">
         <v>0</v>
@@ -890,7 +884,7 @@
         <v/>
       </c>
       <c r="C31" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D31" s="2" t="n">
         <v>0</v>
@@ -905,7 +899,7 @@
         <v/>
       </c>
       <c r="C32" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D32" s="2" t="n">
         <v>0</v>
@@ -920,7 +914,7 @@
         <v/>
       </c>
       <c r="C33" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D33" s="2" t="n">
         <v>0</v>
@@ -935,7 +929,7 @@
         <v/>
       </c>
       <c r="C34" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D34" s="2" t="n">
         <v>0</v>
@@ -950,7 +944,7 @@
         <v/>
       </c>
       <c r="C35" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D35" s="2" t="n">
         <v>0</v>
@@ -965,7 +959,7 @@
         <v/>
       </c>
       <c r="C36" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D36" s="2" t="n">
         <v>0</v>
@@ -980,7 +974,7 @@
         <v/>
       </c>
       <c r="C37" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D37" s="2" t="n">
         <v>0</v>
@@ -995,7 +989,7 @@
         <v/>
       </c>
       <c r="C38" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D38" s="2" t="n">
         <v>0</v>
@@ -1010,7 +1004,7 @@
         <v/>
       </c>
       <c r="C39" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D39" s="2" t="n">
         <v>0</v>
@@ -1025,7 +1019,7 @@
         <v/>
       </c>
       <c r="C40" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D40" s="2" t="n">
         <v>0</v>
@@ -1040,7 +1034,7 @@
         <v/>
       </c>
       <c r="C41" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D41" s="2" t="n">
         <v>0</v>
@@ -1055,7 +1049,7 @@
         <v/>
       </c>
       <c r="C42" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D42" s="2" t="n">
         <v>0</v>
@@ -1070,7 +1064,7 @@
         <v/>
       </c>
       <c r="C43" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D43" s="2" t="n">
         <v>0</v>
@@ -1085,7 +1079,7 @@
         <v/>
       </c>
       <c r="C44" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D44" s="2" t="n">
         <v>0</v>
@@ -1100,7 +1094,7 @@
         <v/>
       </c>
       <c r="C45" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D45" s="2" t="n">
         <v>0</v>
@@ -1115,7 +1109,7 @@
         <v/>
       </c>
       <c r="C46" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D46" s="2" t="n">
         <v>0</v>
@@ -1130,7 +1124,7 @@
         <v/>
       </c>
       <c r="C47" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D47" s="2" t="n">
         <v>0</v>
@@ -1145,7 +1139,7 @@
         <v/>
       </c>
       <c r="C48" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D48" s="2" t="n">
         <v>0</v>
@@ -1160,7 +1154,7 @@
         <v/>
       </c>
       <c r="C49" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D49" s="2" t="n">
         <v>0</v>
@@ -1175,7 +1169,7 @@
         <v/>
       </c>
       <c r="C50" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D50" s="2" t="n">
         <v>0</v>
@@ -1190,7 +1184,7 @@
         <v/>
       </c>
       <c r="C51" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D51" s="2" t="n">
         <v>0</v>
@@ -1205,7 +1199,7 @@
         <v/>
       </c>
       <c r="C52" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D52" s="2" t="n">
         <v>0</v>
@@ -1220,7 +1214,7 @@
         <v/>
       </c>
       <c r="C53" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D53" s="2" t="n">
         <v>0</v>
@@ -1235,7 +1229,7 @@
         <v/>
       </c>
       <c r="C54" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D54" s="2" t="n">
         <v>0</v>
@@ -1250,7 +1244,7 @@
         <v/>
       </c>
       <c r="C55" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D55" s="2" t="n">
         <v>0</v>
@@ -1265,7 +1259,7 @@
         <v/>
       </c>
       <c r="C56" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D56" s="2" t="n">
         <v>0</v>
@@ -1280,7 +1274,7 @@
         <v/>
       </c>
       <c r="C57" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D57" s="2" t="n">
         <v>0</v>
@@ -1295,7 +1289,7 @@
         <v/>
       </c>
       <c r="C58" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D58" s="2" t="n">
         <v>0</v>
@@ -1310,7 +1304,7 @@
         <v/>
       </c>
       <c r="C59" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D59" s="2" t="n">
         <v>0</v>
@@ -1325,7 +1319,7 @@
         <v/>
       </c>
       <c r="C60" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D60" s="2" t="n">
         <v>0</v>
@@ -1340,7 +1334,7 @@
         <v/>
       </c>
       <c r="C61" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D61" s="2" t="n">
         <v>0</v>
@@ -1355,7 +1349,7 @@
         <v/>
       </c>
       <c r="C62" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D62" s="2" t="n">
         <v>0</v>
@@ -1370,7 +1364,7 @@
         <v/>
       </c>
       <c r="C63" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D63" s="2" t="n">
         <v>0</v>
@@ -1385,7 +1379,7 @@
         <v/>
       </c>
       <c r="C64" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D64" s="2" t="n">
         <v>0</v>
@@ -1400,7 +1394,7 @@
         <v/>
       </c>
       <c r="C65" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D65" s="2" t="n">
         <v>0</v>
@@ -1415,7 +1409,7 @@
         <v/>
       </c>
       <c r="C66" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D66" s="2" t="n">
         <v>0</v>
@@ -1430,7 +1424,7 @@
         <v/>
       </c>
       <c r="C67" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D67" s="2" t="n">
         <v>0</v>
@@ -1445,7 +1439,7 @@
         <v/>
       </c>
       <c r="C68" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D68" s="2" t="n">
         <v>0</v>
@@ -1460,7 +1454,7 @@
         <v/>
       </c>
       <c r="C69" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D69" s="2" t="n">
         <v>0</v>
@@ -1475,7 +1469,7 @@
         <v/>
       </c>
       <c r="C70" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D70" s="2" t="n">
         <v>0</v>
@@ -1490,7 +1484,7 @@
         <v/>
       </c>
       <c r="C71" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D71" s="2" t="n">
         <v>0</v>
@@ -1505,7 +1499,7 @@
         <v/>
       </c>
       <c r="C72" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D72" s="2" t="n">
         <v>0</v>
@@ -1520,7 +1514,7 @@
         <v/>
       </c>
       <c r="C73" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D73" s="2" t="n">
         <v>0</v>
@@ -1535,7 +1529,7 @@
         <v/>
       </c>
       <c r="C74" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D74" s="2" t="n">
         <v>0</v>
@@ -1550,7 +1544,7 @@
         <v/>
       </c>
       <c r="C75" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D75" s="2" t="n">
         <v>0</v>
@@ -1565,7 +1559,7 @@
         <v/>
       </c>
       <c r="C76" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D76" s="2" t="n">
         <v>0</v>
@@ -1580,7 +1574,7 @@
         <v/>
       </c>
       <c r="C77" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D77" s="2" t="n">
         <v>0</v>
@@ -1595,7 +1589,7 @@
         <v/>
       </c>
       <c r="C78" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D78" s="2" t="n">
         <v>0</v>
@@ -1610,7 +1604,7 @@
         <v/>
       </c>
       <c r="C79" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D79" s="2" t="n">
         <v>0</v>
@@ -1625,7 +1619,7 @@
         <v/>
       </c>
       <c r="C80" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D80" s="2" t="n">
         <v>0</v>
@@ -1640,7 +1634,7 @@
         <v/>
       </c>
       <c r="C81" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D81" s="2" t="n">
         <v>0</v>
@@ -1655,7 +1649,7 @@
         <v/>
       </c>
       <c r="C82" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D82" s="2" t="n">
         <v>0</v>
@@ -1670,7 +1664,7 @@
         <v/>
       </c>
       <c r="C83" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D83" s="2" t="n">
         <v>0</v>
@@ -1685,7 +1679,7 @@
         <v/>
       </c>
       <c r="C84" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D84" s="2" t="n">
         <v>0</v>
@@ -1700,7 +1694,7 @@
         <v/>
       </c>
       <c r="C85" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D85" s="2" t="n">
         <v>0</v>
@@ -1715,7 +1709,7 @@
         <v/>
       </c>
       <c r="C86" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D86" s="2" t="n">
         <v>0</v>
@@ -1730,7 +1724,7 @@
         <v/>
       </c>
       <c r="C87" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D87" s="2" t="n">
         <v>0</v>
@@ -1745,7 +1739,7 @@
         <v/>
       </c>
       <c r="C88" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D88" s="2" t="n">
         <v>0</v>
@@ -1760,7 +1754,7 @@
         <v/>
       </c>
       <c r="C89" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D89" s="2" t="n">
         <v>0</v>
@@ -1775,7 +1769,7 @@
         <v/>
       </c>
       <c r="C90" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D90" s="2" t="n">
         <v>0</v>
@@ -1790,7 +1784,7 @@
         <v/>
       </c>
       <c r="C91" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D91" s="2" t="n">
         <v>0</v>
@@ -1805,7 +1799,7 @@
         <v/>
       </c>
       <c r="C92" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D92" s="2" t="n">
         <v>0</v>
@@ -1820,7 +1814,7 @@
         <v/>
       </c>
       <c r="C93" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D93" s="2" t="n">
         <v>0</v>
@@ -1835,7 +1829,7 @@
         <v/>
       </c>
       <c r="C94" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D94" s="2" t="n">
         <v>0</v>
@@ -1850,7 +1844,7 @@
         <v/>
       </c>
       <c r="C95" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D95" s="2" t="n">
         <v>0</v>
@@ -1865,7 +1859,7 @@
         <v/>
       </c>
       <c r="C96" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D96" s="2" t="n">
         <v>0</v>
@@ -1880,7 +1874,7 @@
         <v/>
       </c>
       <c r="C97" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D97" s="2" t="n">
         <v>0</v>
@@ -1895,7 +1889,7 @@
         <v/>
       </c>
       <c r="C98" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D98" s="2" t="n">
         <v>0</v>
@@ -1910,7 +1904,7 @@
         <v/>
       </c>
       <c r="C99" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D99" s="2" t="n">
         <v>0</v>
@@ -1925,7 +1919,7 @@
         <v/>
       </c>
       <c r="C100" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D100" s="2" t="n">
         <v>0</v>
@@ -1940,7 +1934,7 @@
         <v/>
       </c>
       <c r="C101" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D101" s="2" t="n">
         <v>0</v>
@@ -1955,7 +1949,7 @@
         <v/>
       </c>
       <c r="C102" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D102" s="2" t="n">
         <v>0</v>
@@ -1970,7 +1964,7 @@
         <v/>
       </c>
       <c r="C103" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D103" s="2" t="n">
         <v>0</v>
@@ -1985,7 +1979,7 @@
         <v/>
       </c>
       <c r="C104" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D104" s="2" t="n">
         <v>0</v>
@@ -2000,7 +1994,7 @@
         <v/>
       </c>
       <c r="C105" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D105" s="2" t="n">
         <v>0</v>
@@ -2015,7 +2009,7 @@
         <v/>
       </c>
       <c r="C106" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D106" s="2" t="n">
         <v>0</v>
@@ -2030,7 +2024,7 @@
         <v/>
       </c>
       <c r="C107" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D107" s="2" t="n">
         <v>0</v>
@@ -2045,7 +2039,7 @@
         <v/>
       </c>
       <c r="C108" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D108" s="2" t="n">
         <v>0</v>
@@ -2060,7 +2054,7 @@
         <v/>
       </c>
       <c r="C109" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D109" s="2" t="n">
         <v>0</v>
@@ -2075,7 +2069,7 @@
         <v/>
       </c>
       <c r="C110" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D110" s="2" t="n">
         <v>0</v>
@@ -2090,7 +2084,7 @@
         <v/>
       </c>
       <c r="C111" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D111" s="2" t="n">
         <v>0</v>
@@ -2105,7 +2099,7 @@
         <v/>
       </c>
       <c r="C112" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D112" s="2" t="n">
         <v>0</v>
@@ -2120,7 +2114,7 @@
         <v/>
       </c>
       <c r="C113" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D113" s="2" t="n">
         <v>0</v>
@@ -2135,7 +2129,7 @@
         <v/>
       </c>
       <c r="C114" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D114" s="2" t="n">
         <v>0</v>
@@ -2150,7 +2144,7 @@
         <v/>
       </c>
       <c r="C115" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D115" s="2" t="n">
         <v>0</v>
@@ -2165,7 +2159,7 @@
         <v/>
       </c>
       <c r="C116" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D116" s="2" t="n">
         <v>0</v>
@@ -2180,7 +2174,7 @@
         <v/>
       </c>
       <c r="C117" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D117" s="2" t="n">
         <v>0</v>
@@ -2195,7 +2189,7 @@
         <v/>
       </c>
       <c r="C118" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D118" s="2" t="n">
         <v>0</v>
@@ -2210,7 +2204,7 @@
         <v/>
       </c>
       <c r="C119" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D119" s="2" t="n">
         <v>0</v>
@@ -2225,7 +2219,7 @@
         <v/>
       </c>
       <c r="C120" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D120" s="2" t="n">
         <v>0</v>
@@ -2240,7 +2234,7 @@
         <v/>
       </c>
       <c r="C121" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D121" s="2" t="n">
         <v>0</v>
@@ -2255,7 +2249,7 @@
         <v/>
       </c>
       <c r="C122" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D122" s="2" t="n">
         <v>0</v>
@@ -2270,7 +2264,7 @@
         <v/>
       </c>
       <c r="C123" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D123" s="2" t="n">
         <v>0</v>
@@ -2285,7 +2279,7 @@
         <v/>
       </c>
       <c r="C124" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D124" s="2" t="n">
         <v>0</v>
@@ -2300,7 +2294,7 @@
         <v/>
       </c>
       <c r="C125" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D125" s="2" t="n">
         <v>0</v>
@@ -2315,7 +2309,7 @@
         <v/>
       </c>
       <c r="C126" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D126" s="2" t="n">
         <v>0</v>
@@ -2330,7 +2324,7 @@
         <v/>
       </c>
       <c r="C127" s="5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D127" s="2" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Write.py [Connected and written]
</commit_message>
<xml_diff>
--- a/parking_lot.xlsx
+++ b/parking_lot.xlsx
@@ -412,15 +412,14 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <f>FALSE()</f>
-        <v/>
+      <c r="B2" s="3" t="b">
+        <v>0</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>123456</v>
+        <v>0</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="3" s="1" spans="1:5">
@@ -585,7 +584,7 @@
         <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>357159</v>
+        <v>123456</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="14" s="1" spans="1:5">
@@ -622,15 +621,14 @@
       <c r="A16" t="n">
         <v>15</v>
       </c>
-      <c r="B16">
-        <f>FALSE()</f>
-        <v/>
+      <c r="B16" t="b">
+        <v>0</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="n">
-        <v>123456</v>
+        <v>0</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="17" s="1" spans="1:5">

</xml_diff>